<commit_message>
Small adjustments to BOM.
</commit_message>
<xml_diff>
--- a/mechanics/Total_BOM_Ver_1_0_final.xlsx
+++ b/mechanics/Total_BOM_Ver_1_0_final.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STEVAL_workspace\workspace\various_documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STEVAL_workspace\workspace\cpcbm_repo_2\mechanics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Totals Frame BOM" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>ISO 7380 M3X4 A2</t>
-  </si>
-  <si>
-    <t>Makerbeam T-nut</t>
   </si>
   <si>
     <t>M3 self-locking nut</t>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>12V 10A power supply</t>
+  </si>
+  <si>
+    <t>Makerbeam T-slot nut</t>
   </si>
 </sst>
 </file>
@@ -935,7 +935,7 @@
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="B7" s="6">
         <v>24</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="6">
         <v>46</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6">
         <v>12</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6">
@@ -1124,7 +1124,7 @@
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="6">
         <v>2</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="6">
         <v>8</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="6">
         <v>4</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
@@ -1225,7 +1225,7 @@
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="6">
         <v>8</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="6">
         <v>16</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="6">
         <v>4</v>
@@ -1323,13 +1323,13 @@
         <v>6</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6">
@@ -1344,13 +1344,13 @@
         <v>2</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1365,13 +1365,13 @@
         <v>2</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1386,13 +1386,13 @@
         <v>2</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="6">
         <v>2</v>
@@ -1407,13 +1407,13 @@
         <v>2</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6">
         <v>2</v>
@@ -1428,13 +1428,13 @@
         <v>2</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6">
@@ -1449,13 +1449,13 @@
         <v>8</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6">
@@ -1470,13 +1470,13 @@
         <v>2</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6">
@@ -1491,13 +1491,13 @@
         <v>2</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6">
@@ -1516,7 +1516,7 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6">
@@ -1535,7 +1535,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6">
@@ -1550,13 +1550,13 @@
         <v>2</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1571,13 +1571,13 @@
         <v>1</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1592,13 +1592,13 @@
         <v>1</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1613,13 +1613,13 @@
         <v>1</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1653,13 +1653,13 @@
         <v>2</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="43" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1693,13 +1693,13 @@
         <v>1</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1714,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1735,13 +1735,13 @@
         <v>1</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1922,7 +1922,7 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="56" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="57" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" s="28"/>
       <c r="C57" s="28"/>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2087,7 +2087,7 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2106,7 +2106,7 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="62" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2135,13 +2135,13 @@
       <c r="G62" s="5"/>
       <c r="H62" s="6"/>
       <c r="I62" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="65" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -2198,7 +2198,7 @@
     </row>
     <row r="66" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -2217,7 +2217,7 @@
     </row>
     <row r="67" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -2234,9 +2234,9 @@
       <c r="I67" s="5"/>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="69" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="70" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>

</xml_diff>